<commit_message>
SDS Test Cases ver 1/SDS test plan ver 1
added test cases and created a test plan for testing and debugging purposes
</commit_message>
<xml_diff>
--- a/SDS_ Test Cases.xlsx
+++ b/SDS_ Test Cases.xlsx
@@ -134,19 +134,24 @@
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
       <t xml:space="preserve">Browser is open to url 
 </t>
     </r>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
         <u/>
       </rPr>
       <t>http://trustyticket.com</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
       <t xml:space="preserve">
 No previous account 
 associated to browser</t>
@@ -171,7 +176,7 @@
   </si>
   <si>
     <t>User_Sign_In
-Theater_User_data
+Theater_User_Data
 Movie_Theater_Page</t>
   </si>
   <si>
@@ -185,19 +190,24 @@
   </si>
   <si>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
       <t xml:space="preserve">Browser open to url 
 </t>
     </r>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
+        <sz val="10.0"/>
         <u/>
       </rPr>
       <t>http://trustyticket</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
       <t>.com
 User acount exists
 User is not signed in</t>
@@ -348,6 +358,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -355,9 +366,21 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -370,18 +393,8 @@
     </font>
     <font>
       <u/>
+      <sz val="10.0"/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="9.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -404,20 +417,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -426,34 +439,31 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -752,12 +762,12 @@
       </c>
     </row>
     <row r="3" ht="26.25" customHeight="1">
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" ht="26.25" customHeight="1">
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -777,7 +787,7 @@
       <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -827,28 +837,28 @@
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -858,28 +868,28 @@
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -889,28 +899,28 @@
       <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -920,28 +930,28 @@
       <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -951,28 +961,28 @@
       <c r="A23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="12" t="s">
         <v>68</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -982,28 +992,28 @@
       <c r="A26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="12" t="s">
         <v>76</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1028,10 +1038,10 @@
       <c r="F29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="H29" s="14" t="s">
         <v>16</v>
       </c>
       <c r="I29" s="5" t="s">

</xml_diff>